<commit_message>
fixed trainer Pokemon modification erros in Emerald
Evolution Array had the following incorrect evolutions:

Roselia -> Spheal
Duskull -> Snorunt
Dusclops -> Glalie
</commit_message>
<xml_diff>
--- a/Gen III.xlsx
+++ b/Gen III.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abzb1\Dropbox\Programs\Level-Recurver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4F3B4F-CD16-4B44-9339-32EB13D19A93}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6555188B-3709-4207-A614-A2F99B7ED99A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1833" windowWidth="25600" windowHeight="11967" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pokemon data" sheetId="1" r:id="rId1"/>
@@ -2022,11 +2022,11 @@
       <sheetName val="Gen III Original Stats"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
       <sheetData sheetId="5">
         <row r="1">
           <cell r="A1" t="str">
@@ -31118,10 +31118,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
       <sheetData sheetId="11"/>
     </sheetDataSet>
   </externalBook>
@@ -31451,8 +31451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -33663,7 +33663,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -34066,8 +34066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{751A757F-64FD-4284-BD62-97222992F7A3}">
   <dimension ref="A1:L402"/>
   <sheetViews>
-    <sheetView topLeftCell="A370" workbookViewId="0">
-      <selection activeCell="I402" sqref="I402"/>
+    <sheetView tabSelected="1" topLeftCell="A371" workbookViewId="0">
+      <selection activeCell="L402" sqref="L402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -50611,15 +50611,14 @@
         <v>16,32,0,16,36,0,16,36,0,7,10,0,7,10,0,18,36,0,20,0,20,0,22,0,100,0,22,0,16,21,0,16,21,0,5,0,50,0,5,0,22,27,21,26,0,24,0,31,0,26,0,28,0,33,0,28,0,5,0,25,30,0,16,21,0,28,33,0,21,26,0,30,0,25,30,0,40,0,37,0,30,35,0,31,0,34,0,38,0,5,0,25,30,0,5,26,0,28,0,30,0,5,0,28,0,0,0,5,35,0,42,47,52,57,0,32,37,33,0,5,0,0,0,0,5,10,0,0,20,0,0,0,0,0,0,0,30,40,0,40,0,0,0,0,0,0,30,55,0,0,0,16,32,0,14,36,0,18,30,0,15,0,20,0,18,0,22,0,0,27,0,10,10,10,10,30,25,0,15,30,0,0,18,0,0,0,18,27,0,40,5,0,5,40,0,0,0,40,0,40,0,0,0,31,0,0,40,0,23,0,0,0,0,0,30,30,0,38,0,33,38,0,25,0,0,0,0,24,0,0,25,0,40,0,0,20,0,30,30,30,0,0,0,0,0,30,55,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,16,36,0,16,36,0,16,36,0,18,0,20,0,7,10,0,10,0,14,19,0,14,19,0,20,0,0,22,0,23,0,0,25,0,22,0,40,0,20,0,0,36,0,30,0,0,30,0,0,30,0,5,0,30,0,35,45,0,24,0,26,0,33,0,32,44,0,32,0,42,0,0,0,15,32,0,0,0,0,37,0,35,0,15,37,</v>
       </c>
       <c r="J362">
-        <f t="shared" si="27"/>
-        <v>346</v>
+        <v>362</v>
       </c>
       <c r="K362" t="s">
         <v>49</v>
       </c>
       <c r="L362" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,</v>
       </c>
     </row>
     <row r="363" spans="1:12" x14ac:dyDescent="0.5">
@@ -50657,15 +50656,14 @@
         <v>16,32,0,16,36,0,16,36,0,7,10,0,7,10,0,18,36,0,20,0,20,0,22,0,100,0,22,0,16,21,0,16,21,0,5,0,50,0,5,0,22,27,21,26,0,24,0,31,0,26,0,28,0,33,0,28,0,5,0,25,30,0,16,21,0,28,33,0,21,26,0,30,0,25,30,0,40,0,37,0,30,35,0,31,0,34,0,38,0,5,0,25,30,0,5,26,0,28,0,30,0,5,0,28,0,0,0,5,35,0,42,47,52,57,0,32,37,33,0,5,0,0,0,0,5,10,0,0,20,0,0,0,0,0,0,0,30,40,0,40,0,0,0,0,0,0,30,55,0,0,0,16,32,0,14,36,0,18,30,0,15,0,20,0,18,0,22,0,0,27,0,10,10,10,10,30,25,0,15,30,0,0,18,0,0,0,18,27,0,40,5,0,5,40,0,0,0,40,0,40,0,0,0,31,0,0,40,0,23,0,0,0,0,0,30,30,0,38,0,33,38,0,25,0,0,0,0,24,0,0,25,0,40,0,0,20,0,30,30,30,0,0,0,0,0,30,55,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,16,36,0,16,36,0,16,36,0,18,0,20,0,7,10,0,10,0,14,19,0,14,19,0,20,0,0,22,0,23,0,0,25,0,22,0,40,0,20,0,0,36,0,30,0,0,30,0,0,30,0,5,0,30,0,35,45,0,24,0,26,0,33,0,32,44,0,32,0,42,0,0,0,15,32,0,0,0,0,37,0,35,0,15,37,42,</v>
       </c>
       <c r="J363">
-        <f t="shared" si="27"/>
-        <v>347</v>
+        <v>362</v>
       </c>
       <c r="K363" t="s">
         <v>49</v>
       </c>
       <c r="L363" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,</v>
       </c>
     </row>
     <row r="364" spans="1:12" x14ac:dyDescent="0.5">
@@ -50703,15 +50701,14 @@
         <v>16,32,0,16,36,0,16,36,0,7,10,0,7,10,0,18,36,0,20,0,20,0,22,0,100,0,22,0,16,21,0,16,21,0,5,0,50,0,5,0,22,27,21,26,0,24,0,31,0,26,0,28,0,33,0,28,0,5,0,25,30,0,16,21,0,28,33,0,21,26,0,30,0,25,30,0,40,0,37,0,30,35,0,31,0,34,0,38,0,5,0,25,30,0,5,26,0,28,0,30,0,5,0,28,0,0,0,5,35,0,42,47,52,57,0,32,37,33,0,5,0,0,0,0,5,10,0,0,20,0,0,0,0,0,0,0,30,40,0,40,0,0,0,0,0,0,30,55,0,0,0,16,32,0,14,36,0,18,30,0,15,0,20,0,18,0,22,0,0,27,0,10,10,10,10,30,25,0,15,30,0,0,18,0,0,0,18,27,0,40,5,0,5,40,0,0,0,40,0,40,0,0,0,31,0,0,40,0,23,0,0,0,0,0,30,30,0,38,0,33,38,0,25,0,0,0,0,24,0,0,25,0,40,0,0,20,0,30,30,30,0,0,0,0,0,30,55,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,16,36,0,16,36,0,16,36,0,18,0,20,0,7,10,0,10,0,14,19,0,14,19,0,20,0,0,22,0,23,0,0,25,0,22,0,40,0,20,0,0,36,0,30,0,0,30,0,0,30,0,5,0,30,0,35,45,0,24,0,26,0,33,0,32,44,0,32,0,42,0,0,0,15,32,0,0,0,0,37,0,35,0,15,37,42,36,</v>
       </c>
       <c r="J364">
-        <f t="shared" si="27"/>
-        <v>341</v>
+        <v>363</v>
       </c>
       <c r="K364" t="s">
         <v>49</v>
       </c>
       <c r="L364" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,</v>
       </c>
     </row>
     <row r="365" spans="1:12" x14ac:dyDescent="0.5">
@@ -50757,7 +50754,7 @@
       </c>
       <c r="L365" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,</v>
       </c>
     </row>
     <row r="366" spans="1:12" x14ac:dyDescent="0.5">
@@ -50803,7 +50800,7 @@
       </c>
       <c r="L366" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,</v>
       </c>
     </row>
     <row r="367" spans="1:12" x14ac:dyDescent="0.5">
@@ -50849,7 +50846,7 @@
       </c>
       <c r="L367" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,</v>
       </c>
     </row>
     <row r="368" spans="1:12" x14ac:dyDescent="0.5">
@@ -50895,7 +50892,7 @@
       </c>
       <c r="L368" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,</v>
       </c>
     </row>
     <row r="369" spans="1:12" x14ac:dyDescent="0.5">
@@ -50941,7 +50938,7 @@
       </c>
       <c r="L369" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,</v>
       </c>
     </row>
     <row r="370" spans="1:12" x14ac:dyDescent="0.5">
@@ -50987,7 +50984,7 @@
       </c>
       <c r="L370" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,</v>
       </c>
     </row>
     <row r="371" spans="1:12" x14ac:dyDescent="0.5">
@@ -51033,7 +51030,7 @@
       </c>
       <c r="L371" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,</v>
       </c>
     </row>
     <row r="372" spans="1:12" x14ac:dyDescent="0.5">
@@ -51079,7 +51076,7 @@
       </c>
       <c r="L372" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,</v>
       </c>
     </row>
     <row r="373" spans="1:12" x14ac:dyDescent="0.5">
@@ -51125,7 +51122,7 @@
       </c>
       <c r="L373" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,</v>
       </c>
     </row>
     <row r="374" spans="1:12" x14ac:dyDescent="0.5">
@@ -51171,7 +51168,7 @@
       </c>
       <c r="L374" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,</v>
       </c>
     </row>
     <row r="375" spans="1:12" x14ac:dyDescent="0.5">
@@ -51217,7 +51214,7 @@
       </c>
       <c r="L375" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,</v>
       </c>
     </row>
     <row r="376" spans="1:12" x14ac:dyDescent="0.5">
@@ -51263,7 +51260,7 @@
       </c>
       <c r="L376" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,</v>
       </c>
     </row>
     <row r="377" spans="1:12" x14ac:dyDescent="0.5">
@@ -51309,7 +51306,7 @@
       </c>
       <c r="L377" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,</v>
       </c>
     </row>
     <row r="378" spans="1:12" x14ac:dyDescent="0.5">
@@ -51355,7 +51352,7 @@
       </c>
       <c r="L378" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,</v>
       </c>
     </row>
     <row r="379" spans="1:12" x14ac:dyDescent="0.5">
@@ -51401,7 +51398,7 @@
       </c>
       <c r="L379" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,</v>
       </c>
     </row>
     <row r="380" spans="1:12" x14ac:dyDescent="0.5">
@@ -51447,7 +51444,7 @@
       </c>
       <c r="L380" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,</v>
       </c>
     </row>
     <row r="381" spans="1:12" x14ac:dyDescent="0.5">
@@ -51493,7 +51490,7 @@
       </c>
       <c r="L381" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,</v>
       </c>
     </row>
     <row r="382" spans="1:12" x14ac:dyDescent="0.5">
@@ -51539,7 +51536,7 @@
       </c>
       <c r="L382" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,</v>
       </c>
     </row>
     <row r="383" spans="1:12" x14ac:dyDescent="0.5">
@@ -51585,7 +51582,7 @@
       </c>
       <c r="L383" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,</v>
       </c>
     </row>
     <row r="384" spans="1:12" x14ac:dyDescent="0.5">
@@ -51631,7 +51628,7 @@
       </c>
       <c r="L384" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,</v>
       </c>
     </row>
     <row r="385" spans="1:12" x14ac:dyDescent="0.5">
@@ -51677,7 +51674,7 @@
       </c>
       <c r="L385" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,</v>
       </c>
     </row>
     <row r="386" spans="1:12" x14ac:dyDescent="0.5">
@@ -51723,7 +51720,7 @@
       </c>
       <c r="L386" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,</v>
       </c>
     </row>
     <row r="387" spans="1:12" x14ac:dyDescent="0.5">
@@ -51769,7 +51766,7 @@
       </c>
       <c r="L387" t="str">
         <f t="shared" si="25"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,</v>
       </c>
     </row>
     <row r="388" spans="1:12" x14ac:dyDescent="0.5">
@@ -51815,7 +51812,7 @@
       </c>
       <c r="L388" t="str">
         <f t="shared" ref="L388:L401" si="31">_xlfn.CONCAT(L387,J388,K388)</f>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,</v>
       </c>
     </row>
     <row r="389" spans="1:12" x14ac:dyDescent="0.5">
@@ -51861,7 +51858,7 @@
       </c>
       <c r="L389" t="str">
         <f t="shared" si="31"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,</v>
       </c>
     </row>
     <row r="390" spans="1:12" x14ac:dyDescent="0.5">
@@ -51907,7 +51904,7 @@
       </c>
       <c r="L390" t="str">
         <f t="shared" si="31"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,</v>
       </c>
     </row>
     <row r="391" spans="1:12" x14ac:dyDescent="0.5">
@@ -51953,7 +51950,7 @@
       </c>
       <c r="L391" t="str">
         <f t="shared" si="31"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,</v>
       </c>
     </row>
     <row r="392" spans="1:12" x14ac:dyDescent="0.5">
@@ -51999,7 +51996,7 @@
       </c>
       <c r="L392" t="str">
         <f t="shared" si="31"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,</v>
       </c>
     </row>
     <row r="393" spans="1:12" x14ac:dyDescent="0.5">
@@ -52045,7 +52042,7 @@
       </c>
       <c r="L393" t="str">
         <f t="shared" si="31"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,393,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,393,</v>
       </c>
     </row>
     <row r="394" spans="1:12" x14ac:dyDescent="0.5">
@@ -52091,7 +52088,7 @@
       </c>
       <c r="L394" t="str">
         <f t="shared" si="31"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,393,394,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,393,394,</v>
       </c>
     </row>
     <row r="395" spans="1:12" x14ac:dyDescent="0.5">
@@ -52137,7 +52134,7 @@
       </c>
       <c r="L395" t="str">
         <f t="shared" si="31"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,393,394,394,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,393,394,394,</v>
       </c>
     </row>
     <row r="396" spans="1:12" x14ac:dyDescent="0.5">
@@ -52183,7 +52180,7 @@
       </c>
       <c r="L396" t="str">
         <f t="shared" si="31"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,393,394,394,396,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,393,394,394,396,</v>
       </c>
     </row>
     <row r="397" spans="1:12" x14ac:dyDescent="0.5">
@@ -52229,7 +52226,7 @@
       </c>
       <c r="L397" t="str">
         <f t="shared" si="31"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,393,394,394,396,397,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,393,394,394,396,397,</v>
       </c>
     </row>
     <row r="398" spans="1:12" x14ac:dyDescent="0.5">
@@ -52275,7 +52272,7 @@
       </c>
       <c r="L398" t="str">
         <f t="shared" si="31"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,393,394,394,396,397,397,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,393,394,394,396,397,397,</v>
       </c>
     </row>
     <row r="399" spans="1:12" x14ac:dyDescent="0.5">
@@ -52321,7 +52318,7 @@
       </c>
       <c r="L399" t="str">
         <f t="shared" si="31"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,393,394,394,396,397,397,399,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,393,394,394,396,397,397,399,</v>
       </c>
     </row>
     <row r="400" spans="1:12" x14ac:dyDescent="0.5">
@@ -52367,7 +52364,7 @@
       </c>
       <c r="L400" t="str">
         <f t="shared" si="31"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,393,394,394,396,397,397,399,400,</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,393,394,394,396,397,397,399,400,</v>
       </c>
     </row>
     <row r="401" spans="1:12" x14ac:dyDescent="0.5">
@@ -52406,7 +52403,7 @@
       </c>
       <c r="L401" t="str">
         <f t="shared" si="31"/>
-        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,393,394,394,396,397,397,399,400,400]</v>
+        <v>2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,393,394,394,396,397,397,399,400,400]</v>
       </c>
     </row>
     <row r="402" spans="1:12" x14ac:dyDescent="0.5">
@@ -52420,7 +52417,7 @@
       </c>
       <c r="L402" t="str">
         <f>_xlfn.CONCAT("[",0,",",L401)</f>
-        <v>[0,2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,346,347,341,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,393,394,394,396,397,397,399,400,400]</v>
+        <v>[0,2,3,3,5,6,6,8,9,9,11,12,12,14,15,15,17,18,18,20,20,22,22,24,24,26,26,28,28,30,31,31,33,34,34,36,36,38,38,40,40,42,169,44,45,45,47,47,49,49,51,51,53,53,55,55,57,57,59,59,61,62,62,64,65,65,67,68,68,70,71,71,73,73,75,76,76,78,78,80,80,82,82,83,85,85,87,87,89,89,91,91,93,94,94,208,97,97,99,99,101,101,103,103,105,105,106,107,108,110,110,112,112,242,114,115,117,230,119,119,121,121,122,123,124,125,162,127,128,130,130,131,132,134,134,135,136,137,139,139,141,141,142,143,144,145,146,148,149,149,150,151,153,154,154,156,157,157,159,160,160,162,162,164,164,166,166,168,168,169,171,171,25,35,39,175,176,178,178,180,181,181,182,184,184,185,186,188,189,189,190,192,192,193,195,195,196,197,198,199,200,201,202,203,205,205,206,207,208,210,210,211,212,213,214,215,217,217,219,219,220,221,222,224,224,225,226,227,229,229,230,232,232,233,234,235,237,237,124,125,126,241,242,243,244,245,247,248,248,249,250,251,252,253,254,255,256,257,258,259,260,261,262,263,264,265,266,267,268,269,270,271,272,273,274,275,276,278,279,279,281,282,282,284,285,285,287,287,289,289,291,292,292,294,294,296,297,297,299,300,300,302,302,303,305,305,307,307,308,310,310,312,312,314,314,316,316,317,319,319,313,321,322,324,324,325,327,327,329,329,331,331,333,334,334,336,336,338,338,340,340,342,343,343,345,345,347,347,348,349,12,352,352,353,354,355,357,357,359,359,202,362,362,363,365,366,366,368,368,369,371,372,372,374,374,375,376,378,378,379,380,381,383,384,384,385,386,387,389,389,391,391,393,394,394,396,397,397,399,400,400]</v>
       </c>
     </row>
   </sheetData>

</xml_diff>